<commit_message>
Updates CEDS code tracker.
</commit_message>
<xml_diff>
--- a/documentation/CEDS_Code_Change_Tracker.xlsx
+++ b/documentation/CEDS_Code_Change_Tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="3060" windowWidth="21600" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="17980" yWindow="1320" windowWidth="21600" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
   <si>
     <t>Change name of output from C4.3proc_NC_EF.R (change from E.[em]_total_scaled_EF.csv to C.[em]_total_scaled_EF.csv. Change documentation and makefile to reflect update</t>
   </si>
@@ -367,6 +367,21 @@
   </si>
   <si>
     <t>Remove automaticall install libraries</t>
+  </si>
+  <si>
+    <t>move to Github</t>
+  </si>
+  <si>
+    <t>Change automatic wd to find /CEDS/input</t>
+  </si>
+  <si>
+    <t>Initial move to github</t>
+  </si>
+  <si>
+    <t>2a8f9bb</t>
+  </si>
+  <si>
+    <t>Adds and fixes .gitignore files</t>
   </si>
 </sst>
 </file>
@@ -448,12 +463,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -474,7 +495,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -482,8 +503,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -576,14 +607,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -918,11 +962,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I66" sqref="I66"/>
+      <pane ySplit="2" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2561,6 +2605,88 @@
         <v>6263</v>
       </c>
     </row>
+    <row r="64" spans="1:9" ht="26">
+      <c r="A64" s="30"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="9">
+        <v>60</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="7">
+        <v>42244</v>
+      </c>
+      <c r="G65" s="7">
+        <v>42244</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="9">
+        <v>62</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="7">
+        <v>42247</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G66" s="7">
+        <v>42247</v>
+      </c>
+      <c r="H66" s="9">
+        <v>4611149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="9">
+        <v>63</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="7">
+        <v>42247</v>
+      </c>
+      <c r="G67" s="7">
+        <v>42247</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Updated code change tracker
Updated code change tracker (note: no revision number- uncertain where
to find the codes being used for GitHub revision #s)
</commit_message>
<xml_diff>
--- a/documentation/CEDS_Code_Change_Tracker.xlsx
+++ b/documentation/CEDS_Code_Change_Tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13800" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="111">
   <si>
     <t>Created C.proc_emissions.R to reformat process emissions data, calculate default emissions factors, and combine them with their combustion counterparts.</t>
   </si>
@@ -401,21 +401,22 @@
   </si>
   <si>
     <t>Added buildCEDSTemplate() to data_functions.R</t>
+  </si>
+  <si>
+    <t>Added small changes to IO_functions.R and data_functions.R that were not committed before the semester began.</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yy;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -516,10 +517,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -946,26 +947,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
+      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="48.625" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="9" customWidth="1"/>
     <col min="4" max="6" width="11" style="9"/>
-    <col min="7" max="7" width="12.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="9" customWidth="1"/>
     <col min="8" max="8" width="12" style="9" customWidth="1"/>
     <col min="9" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -976,7 +977,7 @@
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
     </row>
-    <row r="2" spans="1:9" ht="37" thickBot="1">
+    <row r="2" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="52">
+    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>5830</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="52.5" customHeight="1">
+    <row r="4" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
@@ -1054,7 +1055,7 @@
         <v>5831</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26">
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>52</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>5701</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" ht="50.25" customHeight="1">
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>97</v>
       </c>
@@ -1107,7 +1108,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" ht="55.5" customHeight="1">
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>5623</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="48.75" customHeight="1">
+    <row r="8" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="65.25" customHeight="1">
+    <row r="9" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>53</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>5657</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="63" customHeight="1">
+    <row r="10" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>54</v>
       </c>
@@ -1211,7 +1212,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39">
+    <row r="11" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>96</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="39">
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>70</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>5858</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="26">
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>71</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>5874</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="52">
+    <row r="14" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>40</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="53.25" customHeight="1">
+    <row r="15" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>60</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>5890</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="51" customHeight="1">
+    <row r="16" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>24</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30.75" customHeight="1">
+    <row r="17" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>25</v>
       </c>
@@ -1393,7 +1394,7 @@
         <v>5946</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45.75" customHeight="1">
+    <row r="18" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>64</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>5915</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="39">
+    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>68</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>5934</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="78">
+    <row r="20" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>69</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="54.75" customHeight="1">
+    <row r="21" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>82</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="35.25" customHeight="1">
+    <row r="22" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>83</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="38.25" customHeight="1">
+    <row r="23" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>72</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>5977</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="51" customHeight="1">
+    <row r="24" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>73</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>5946</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="67.5" customHeight="1">
+    <row r="25" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>42</v>
       </c>
@@ -1601,7 +1602,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="68.25" customHeight="1">
+    <row r="26" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>41</v>
       </c>
@@ -1627,7 +1628,7 @@
         <v>5978</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="38.25" customHeight="1">
+    <row r="27" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>5</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="104.25" customHeight="1">
+    <row r="29" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>43</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="96" customHeight="1">
+    <row r="30" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>61</v>
       </c>
@@ -1731,7 +1732,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="60.75" customHeight="1">
+    <row r="31" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>95</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>5993</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="39" customHeight="1">
+    <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>51</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>5998</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="42.75" customHeight="1">
+    <row r="33" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>63</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>6030</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="31.5" customHeight="1">
+    <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>66</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>6030</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1">
+    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>67</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>6036</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="41.25" customHeight="1">
+    <row r="36" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>76</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="36" customHeight="1">
+    <row r="37" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>78</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="13" customFormat="1" ht="27" customHeight="1">
+    <row r="38" spans="1:8" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>106</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="93" customHeight="1">
+    <row r="39" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>19</v>
       </c>
@@ -1965,7 +1966,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="37.5" customHeight="1">
+    <row r="40" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>79</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="40.5" customHeight="1">
+    <row r="41" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>80</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>6080</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="47.25" customHeight="1">
+    <row r="42" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>107</v>
       </c>
@@ -2043,7 +2044,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="27.75" customHeight="1">
+    <row r="43" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>108</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="53.25" customHeight="1">
+    <row r="44" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>74</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="16" customFormat="1" ht="52">
+    <row r="45" spans="1:8" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>28</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="17" customFormat="1" ht="26">
+    <row r="46" spans="1:8" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>55</v>
       </c>
@@ -2147,7 +2148,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="15" customFormat="1" ht="53.25" customHeight="1">
+    <row r="47" spans="1:8" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>101</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>6137</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="18" customFormat="1" ht="53.25" customHeight="1">
+    <row r="48" spans="1:8" s="18" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>57</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>6137</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="19" customFormat="1" ht="50.25" customHeight="1">
+    <row r="49" spans="1:9" s="19" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>31</v>
       </c>
@@ -2225,7 +2226,7 @@
         <v>6142</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="26">
+    <row r="50" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>58</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>6145</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="52">
+    <row r="51" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>29</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>6145</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="54" customHeight="1">
+    <row r="52" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>32</v>
       </c>
@@ -2304,7 +2305,7 @@
       </c>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="39">
+    <row r="53" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>20</v>
       </c>
@@ -2330,7 +2331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>21</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="39">
+    <row r="55" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>1</v>
       </c>
@@ -2382,7 +2383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="49.5" customHeight="1">
+    <row r="56" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>26</v>
       </c>
@@ -2408,7 +2409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="26">
+    <row r="57" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>14</v>
       </c>
@@ -2434,7 +2435,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="52">
+    <row r="58" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>4</v>
       </c>
@@ -2460,7 +2461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>103</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>6230</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="26">
+    <row r="60" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>34</v>
       </c>
@@ -2512,7 +2513,7 @@
         <v>6254</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="44.25" customHeight="1">
+    <row r="61" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>35</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>6258</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="33" customHeight="1">
+    <row r="62" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
         <v>36</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>6260</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>85</v>
       </c>
@@ -2590,7 +2591,7 @@
         <v>6263</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="26">
+    <row r="64" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" s="29"/>
       <c r="B64" s="29"/>
       <c r="C64" s="29"/>
@@ -2603,7 +2604,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>88</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>87</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>4611149</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>90</v>
       </c>
@@ -2672,7 +2673,7 @@
         <v>42247</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>91</v>
       </c>
@@ -2698,8 +2699,33 @@
         <v>18</v>
       </c>
     </row>
+    <row r="69" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="9">
+        <v>65</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="7">
+        <v>42262</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G69" s="7">
+        <v>42262</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:G1"/>

</xml_diff>

<commit_message>
Update code tracker, fix typo in documentation.
</commit_message>
<xml_diff>
--- a/documentation/CEDS_Code_Change_Tracker.xlsx
+++ b/documentation/CEDS_Code_Change_Tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
+    <workbookView xWindow="21760" yWindow="6000" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="125">
   <si>
     <t>Created C.proc_emissions.R to reformat process emissions data, calculate default emissions factors, and combine them with their combustion counterparts.</t>
   </si>
@@ -428,6 +428,27 @@
   </si>
   <si>
     <t>fe5e0c3</t>
+  </si>
+  <si>
+    <t>Add Gains SO2 emission Factors</t>
+  </si>
+  <si>
+    <t>Rachel Hoesly, Ryan Bolt</t>
+  </si>
+  <si>
+    <t>0eca975</t>
+  </si>
+  <si>
+    <t>1d8164c</t>
+  </si>
+  <si>
+    <t>deb5b9a</t>
+  </si>
+  <si>
+    <t>rewrite addToEFDb, old function retained in code</t>
+  </si>
+  <si>
+    <t>Add sulfer retention correction to SO2 emission factors (GAINS)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -565,8 +586,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -671,14 +698,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -687,6 +717,9 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -695,6 +728,9 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1029,11 +1065,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
+      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1048,15 +1084,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:9" ht="37" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -2871,7 +2907,7 @@
       <c r="E72" s="7">
         <v>42269</v>
       </c>
-      <c r="G72" s="35">
+      <c r="G72" s="34">
         <v>42269</v>
       </c>
       <c r="H72" s="32" t="s">
@@ -2902,6 +2938,75 @@
       </c>
       <c r="H73" s="31" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="26">
+      <c r="A74" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="9">
+        <v>70</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D74" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="7">
+        <v>42272</v>
+      </c>
+      <c r="G74" s="7">
+        <v>42272</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B75" s="33">
+        <v>71</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="7">
+        <v>42273</v>
+      </c>
+      <c r="G75" s="7">
+        <v>42273</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="26">
+      <c r="A76" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" s="33">
+        <v>72</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="7">
+        <v>42274</v>
+      </c>
+      <c r="G76" s="7">
+        <v>42274</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added full function descriptions
Added full function description to all multi-line functions in
IO_functions.R, analysis_functions.R, and data_functions.R.
</commit_message>
<xml_diff>
--- a/documentation/CEDS_Code_Change_Tracker.xlsx
+++ b/documentation/CEDS_Code_Change_Tracker.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22800" yWindow="1720" windowWidth="17060" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="22800" yWindow="1725" windowWidth="17055" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="134">
   <si>
     <t>Created C.proc_emissions.R to reformat process emissions data, calculate default emissions factors, and combine them with their combustion counterparts.</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>add canada to scaling module</t>
+  </si>
+  <si>
+    <t>Added full function description to all multi-line functions in IO_functions.R, analysis_functions.R, and data_functions.R</t>
   </si>
 </sst>
 </file>
@@ -1111,25 +1114,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
+      <pane ySplit="2" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="48.625" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="9" customWidth="1"/>
     <col min="4" max="6" width="11" style="9"/>
-    <col min="7" max="7" width="12.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="9" customWidth="1"/>
     <col min="8" max="8" width="12" style="9" customWidth="1"/>
     <col min="9" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37"/>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1140,7 +1143,7 @@
       <c r="F1" s="38"/>
       <c r="G1" s="38"/>
     </row>
-    <row r="2" spans="1:9" ht="37" thickBot="1">
+    <row r="2" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="52">
+    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>5830</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="52.5" customHeight="1">
+    <row r="4" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>5831</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26">
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>52</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>5701</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" ht="50.25" customHeight="1">
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>97</v>
       </c>
@@ -1271,7 +1274,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" ht="55.5" customHeight="1">
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>5623</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="48.75" customHeight="1">
+    <row r="8" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="65.25" customHeight="1">
+    <row r="9" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>53</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>5657</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="63" customHeight="1">
+    <row r="10" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>54</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39">
+    <row r="11" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>96</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="39">
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>70</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>5858</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="26">
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>71</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>5874</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="52">
+    <row r="14" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>40</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="53.25" customHeight="1">
+    <row r="15" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>60</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>5890</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="51" customHeight="1">
+    <row r="16" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>24</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30.75" customHeight="1">
+    <row r="17" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>25</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>5946</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45.75" customHeight="1">
+    <row r="18" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>64</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>5915</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="39">
+    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>68</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>5934</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="78">
+    <row r="20" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>69</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="54.75" customHeight="1">
+    <row r="21" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>82</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="35.25" customHeight="1">
+    <row r="22" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>83</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="38.25" customHeight="1">
+    <row r="23" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>72</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>5977</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="51" customHeight="1">
+    <row r="24" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>73</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>5946</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="67.5" customHeight="1">
+    <row r="25" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>42</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="68.25" customHeight="1">
+    <row r="26" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>41</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>5978</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="38.25" customHeight="1">
+    <row r="27" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>5</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="104.25" customHeight="1">
+    <row r="29" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>43</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="96" customHeight="1">
+    <row r="30" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>61</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="60.75" customHeight="1">
+    <row r="31" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>95</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>5993</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="39" customHeight="1">
+    <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>51</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>5998</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="42.75" customHeight="1">
+    <row r="33" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>63</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>6030</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="31.5" customHeight="1">
+    <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>66</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>6030</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1">
+    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>67</v>
       </c>
@@ -2025,7 +2028,7 @@
         <v>6036</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="41.25" customHeight="1">
+    <row r="36" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>76</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="36" customHeight="1">
+    <row r="37" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>78</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="13" customFormat="1" ht="27" customHeight="1">
+    <row r="38" spans="1:8" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>106</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="93" customHeight="1">
+    <row r="39" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>19</v>
       </c>
@@ -2129,7 +2132,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="37.5" customHeight="1">
+    <row r="40" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>79</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="40.5" customHeight="1">
+    <row r="41" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>80</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>6080</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="47.25" customHeight="1">
+    <row r="42" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>107</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="27.75" customHeight="1">
+    <row r="43" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>108</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="53.25" customHeight="1">
+    <row r="44" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>74</v>
       </c>
@@ -2259,7 +2262,7 @@
         <v>6111</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="16" customFormat="1" ht="52">
+    <row r="45" spans="1:8" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>28</v>
       </c>
@@ -2285,7 +2288,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="17" customFormat="1" ht="26">
+    <row r="46" spans="1:8" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>55</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="15" customFormat="1" ht="53.25" customHeight="1">
+    <row r="47" spans="1:8" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>101</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>6137</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="18" customFormat="1" ht="53.25" customHeight="1">
+    <row r="48" spans="1:8" s="18" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>57</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>6137</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="19" customFormat="1" ht="50.25" customHeight="1">
+    <row r="49" spans="1:9" s="19" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>31</v>
       </c>
@@ -2389,7 +2392,7 @@
         <v>6142</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="26">
+    <row r="50" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>58</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>6145</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="52">
+    <row r="51" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>29</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>6145</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="54" customHeight="1">
+    <row r="52" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>32</v>
       </c>
@@ -2468,7 +2471,7 @@
       </c>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="39">
+    <row r="53" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>20</v>
       </c>
@@ -2494,7 +2497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>21</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="39">
+    <row r="55" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>1</v>
       </c>
@@ -2546,7 +2549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="49.5" customHeight="1">
+    <row r="56" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>26</v>
       </c>
@@ -2572,7 +2575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="26">
+    <row r="57" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>14</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>6224</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="52">
+    <row r="58" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>4</v>
       </c>
@@ -2624,7 +2627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>103</v>
       </c>
@@ -2650,7 +2653,7 @@
         <v>6230</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="26">
+    <row r="60" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>34</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>6254</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="44.25" customHeight="1">
+    <row r="61" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>35</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>6258</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="33" customHeight="1">
+    <row r="62" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
         <v>36</v>
       </c>
@@ -2728,7 +2731,7 @@
         <v>6260</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>85</v>
       </c>
@@ -2754,7 +2757,7 @@
         <v>6263</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="26">
+    <row r="64" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" s="29"/>
       <c r="B64" s="29"/>
       <c r="C64" s="29"/>
@@ -2767,7 +2770,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>88</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>87</v>
       </c>
@@ -2816,7 +2819,7 @@
         <v>4611149</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>90</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>42247</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>91</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="31" customFormat="1" ht="26">
+    <row r="69" spans="1:8" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A69" s="31" t="s">
         <v>114</v>
       </c>
@@ -2888,7 +2891,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="39">
+    <row r="70" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>109</v>
       </c>
@@ -2914,7 +2917,7 @@
         <v>8768403</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>110</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>111</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>116</v>
       </c>
@@ -2986,7 +2989,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="26">
+    <row r="74" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>118</v>
       </c>
@@ -3012,7 +3015,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>123</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="26">
+    <row r="76" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>124</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>125</v>
       </c>
@@ -3090,7 +3093,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="26">
+    <row r="78" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>127</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="26">
+    <row r="79" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>128</v>
       </c>
@@ -3142,7 +3145,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>132</v>
       </c>
@@ -3166,6 +3169,29 @@
       </c>
       <c r="H80" s="9" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" s="9">
+        <v>77</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="7">
+        <v>42276</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G81" s="7">
+        <v>42276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Code Change Tracker
</commit_message>
<xml_diff>
--- a/documentation/CEDS_Code_Change_Tracker.xlsx
+++ b/documentation/CEDS_Code_Change_Tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22460" yWindow="2180" windowWidth="17120" windowHeight="13800" tabRatio="500"/>
+    <workbookView xWindow="22540" yWindow="1540" windowWidth="17120" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="168">
   <si>
     <t>Created "header.R" and re-worked all scripts' section 0 to use its functions instead of calling all script startup functions manually.</t>
   </si>
@@ -566,6 +566,21 @@
   </si>
   <si>
     <t>Modifies module B to calculate emission factors by EF parameters (base EF and control percent - and sulfur content and ash retention for SO2).</t>
+  </si>
+  <si>
+    <t>b0a6d6</t>
+  </si>
+  <si>
+    <t>Mod A - Fixes energy as driver data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updates addtoDB function, makes faster </t>
+  </si>
+  <si>
+    <t>bacbd3</t>
+  </si>
+  <si>
+    <t>0f6b74f</t>
   </si>
 </sst>
 </file>
@@ -573,7 +588,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -685,7 +700,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -709,17 +724,21 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -845,11 +864,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -861,6 +883,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -872,6 +896,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1206,11 +1232,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
+      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1225,15 +1251,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A1" s="43"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:9" ht="37" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -3601,6 +3627,75 @@
       </c>
       <c r="H94" s="42" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" s="43">
+        <v>91</v>
+      </c>
+      <c r="C95" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D95" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="7">
+        <v>42342</v>
+      </c>
+      <c r="G95" s="7">
+        <v>42342</v>
+      </c>
+      <c r="H95" s="43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B96" s="43">
+        <v>92</v>
+      </c>
+      <c r="C96" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D96" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="7">
+        <v>42345</v>
+      </c>
+      <c r="G96" s="7">
+        <v>42345</v>
+      </c>
+      <c r="H96" s="43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B97" s="43">
+        <v>93</v>
+      </c>
+      <c r="C97" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D97" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="7">
+        <v>42346</v>
+      </c>
+      <c r="G97" s="7">
+        <v>42346</v>
+      </c>
+      <c r="H97" s="43" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to code change tracker
</commit_message>
<xml_diff>
--- a/documentation/CEDS_Code_Change_Tracker.xlsx
+++ b/documentation/CEDS_Code_Change_Tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="13800" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21600" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="173">
   <si>
     <t>Remove automaticall install libraries</t>
   </si>
@@ -587,21 +587,25 @@
   </si>
   <si>
     <t>ed989b7</t>
+  </si>
+  <si>
+    <t>Minor spacing corrections and phrasing changes made to Makefile comments</t>
+  </si>
+  <si>
+    <t>Added instantiation of "scripts" variable before conditionals to determine child scripts to execute in F1.1.inventory_scaling.R, to avoid errors during execution for BC emissions</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -704,12 +708,6 @@
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -844,6 +842,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1183,2501 +1187,2535 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H98" sqref="H98"/>
+      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="11" customWidth="1"/>
-    <col min="4" max="6" width="11" style="11"/>
-    <col min="7" max="7" width="12.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="11" style="11"/>
+    <col min="1" max="1" width="48.625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="9" customWidth="1"/>
+    <col min="4" max="6" width="11" style="9"/>
+    <col min="7" max="7" width="12.625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="37" thickBot="1">
-      <c r="A2" s="3" t="s">
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="52">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="D3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="6">
         <v>41939</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>42118</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>42135</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>5830</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="52.5" customHeight="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="D4" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="6">
         <v>41939</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>42118</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>42135</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>5831</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="D5" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="7">
         <v>42012</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>42019</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>42046</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>5701</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="9">
+      <c r="C6" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="7">
         <v>42012</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>42072</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>42086</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>5754</v>
       </c>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="C7" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="7">
         <v>42016</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G7" s="9">
+      <c r="F7" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="7">
         <v>42016</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>5623</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="48.75" customHeight="1">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="C8" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="7">
         <v>42016</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>42179</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>42194</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="65.25" customHeight="1">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>7</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="C9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="7">
         <v>42024</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>42026</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>42037</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <v>5657</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="63" customHeight="1">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="D10" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="7">
         <v>42037</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="F10" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="7">
         <v>42046</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <v>5700</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="9">
         <v>9</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="D11" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="7">
         <v>42037</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="9">
+      <c r="F11" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="7">
         <v>42046</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <v>5700</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="39">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="9">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="C12" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="7">
         <v>42156</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="F12" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="7">
         <v>42156</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="9">
         <v>5858</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="26">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>11</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="C13" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="7">
         <v>42159</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>42159</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <v>42159</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="9">
         <v>5874</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="52">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>12</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="9">
+      <c r="C14" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="7">
         <v>42156</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>42179</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>42194</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="53.25" customHeight="1">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="18">
         <v>13</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="C15" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="7">
         <v>42164</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="F15" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="7">
         <v>42164</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="9">
         <v>5890</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="51" customHeight="1">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="18">
         <v>14</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="C16" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="7">
         <v>42171</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="9">
+      <c r="F16" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="7">
         <v>42172</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="18">
         <v>15</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="C17" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="7">
         <v>42171</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>42179</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="7">
         <v>42180</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="9">
         <v>5946</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45.75" customHeight="1">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="18">
         <v>16</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="C18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" s="7">
         <v>42171</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" s="9">
+      <c r="F18" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="7">
         <v>42171</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="9">
         <v>5915</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="39">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="18">
         <v>17</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E19" s="9">
+      <c r="C19" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="7">
         <v>42174</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" s="9">
+      <c r="F19" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="7">
         <v>42178</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="9">
         <v>5934</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="78">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="18">
         <v>18</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="9">
+      <c r="C20" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="7">
         <v>42174</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>42178</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>42194</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="54.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="18">
         <v>19</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="9">
+      <c r="C21" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="7">
         <v>42178</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G21" s="9">
+      <c r="F21" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="7">
         <v>42178</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="18">
         <v>20</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E22" s="9">
+      <c r="C22" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="7">
         <v>42178</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>42179</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>42194</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>21</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E23" s="9">
+      <c r="C23" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="7">
         <v>42179</v>
       </c>
-      <c r="F23" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" s="9">
+      <c r="F23" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="7">
         <v>42192</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="9">
         <v>5977</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="51" customHeight="1">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>22</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" s="9">
+      <c r="C24" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="7">
         <v>42180</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>42180</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="7">
         <v>42180</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="9">
         <v>5946</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="67.5" customHeight="1">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="18">
         <v>23</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="9">
+      <c r="C25" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="7">
         <v>42179</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="9">
+      <c r="F25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="7">
         <v>42194</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="68.25" customHeight="1">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="18">
         <v>24</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E26" s="9">
+      <c r="C26" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="7">
         <v>42180</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="F26" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" s="7">
         <v>42192</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="9">
         <v>5978</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="18">
         <v>25</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E27" s="9">
+      <c r="C27" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E27" s="7">
         <v>42184</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="9">
+      <c r="F27" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="7">
         <v>42194</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="11" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="18">
         <v>26</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E28" s="9">
+      <c r="C28" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="7">
         <v>42187</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="7">
         <v>42187</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>42187</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="104.25" customHeight="1">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="18">
         <v>27</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E29" s="9">
+      <c r="C29" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="7">
         <v>42187</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>42192</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>42194</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="96" customHeight="1">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="18">
         <v>28</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E30" s="9">
+      <c r="C30" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="7">
         <v>42193</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G30" s="9">
+      <c r="F30" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="7">
         <v>42194</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A31" s="12" t="s">
+    <row r="31" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="18">
         <v>29</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E31" s="9">
+      <c r="D31" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="7">
         <v>42175</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>42192</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>42193</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="9">
         <v>5993</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="39" customHeight="1">
-      <c r="A32" s="12" t="s">
+    <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="18">
         <v>30</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E32" s="9">
+      <c r="C32" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="7">
         <v>42194</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G32" s="9">
+      <c r="F32" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="7">
         <v>42194</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="9">
         <v>5998</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="42.75" customHeight="1">
-      <c r="A33" s="11" t="s">
+    <row r="33" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="5">
         <v>31</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E33" s="9">
+      <c r="C33" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E33" s="7">
         <v>42194</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G33" s="9">
+      <c r="F33" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" s="7">
         <v>42198</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="9">
         <v>6030</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="5">
         <v>32</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E34" s="9">
+      <c r="C34" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34" s="7">
         <v>42198</v>
       </c>
-      <c r="F34" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G34" s="9">
+      <c r="F34" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="7">
         <v>42198</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="9">
         <v>6030</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="18">
         <v>33</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E35" s="9">
+      <c r="C35" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="7">
         <v>42199</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="F35" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" s="7">
         <v>42199</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="9">
         <v>6036</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="41.25" customHeight="1">
-      <c r="A36" s="11" t="s">
+    <row r="36" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="18">
         <v>34</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E36" s="9">
+      <c r="D36" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" s="7">
         <v>42199</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36" s="7">
         <v>42201</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <v>42212</v>
       </c>
-      <c r="H36" s="26" t="s">
+      <c r="H36" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="36" customHeight="1">
-      <c r="A37" s="11" t="s">
+    <row r="37" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" s="18">
         <v>35</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E37" s="9">
+      <c r="C37" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" s="7">
         <v>42202</v>
       </c>
-      <c r="F37" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G37" s="9" t="s">
+      <c r="F37" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="15" customFormat="1" ht="27" customHeight="1">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:8" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="18">
         <v>36</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="E38" s="9">
+      <c r="C38" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E38" s="7">
         <v>42202</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="G38" s="9">
+      <c r="F38" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" s="7">
         <v>42212</v>
       </c>
-      <c r="H38" s="16">
+      <c r="H38" s="14">
         <v>6111</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="93" customHeight="1">
-      <c r="A39" s="11" t="s">
+    <row r="39" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B39" s="18">
         <v>37</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E39" s="9">
+      <c r="C39" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="7">
         <v>42202</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39" s="7">
         <v>42207</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="7">
         <v>42212</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="14">
         <v>6111</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A40" s="11" t="s">
+    <row r="40" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" s="18">
         <v>38</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" s="9">
+      <c r="C40" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="7">
         <v>42202</v>
       </c>
-      <c r="F40" s="9">
+      <c r="F40" s="7">
         <v>42202</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="H40" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A41" s="11" t="s">
+    <row r="41" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="20">
+      <c r="B41" s="18">
         <v>39</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E41" s="9">
+      <c r="C41" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" s="7">
         <v>42200</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F41" s="7">
         <v>42200</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="7">
         <v>42197</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="9">
         <v>6080</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="47.25" customHeight="1">
-      <c r="A42" s="11" t="s">
+    <row r="42" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" s="18">
         <v>40</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="9">
+      <c r="C42" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" s="7">
         <v>42208</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42" s="7">
         <v>42212</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="7">
         <v>42212</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="9">
         <v>6111</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A43" s="11" t="s">
+    <row r="43" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="5">
         <v>41</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="9">
+      <c r="C43" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="7">
         <v>42208</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43" s="7">
         <v>42212</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="7">
         <v>42212</v>
       </c>
-      <c r="H43" s="16">
+      <c r="H43" s="14">
         <v>6111</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="5">
         <v>42</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E44" s="9">
+      <c r="C44" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E44" s="7">
         <v>42209</v>
       </c>
-      <c r="F44" s="9">
+      <c r="F44" s="7">
         <v>42212</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="7">
         <v>42212</v>
       </c>
-      <c r="H44" s="16">
+      <c r="H44" s="14">
         <v>6111</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="18" customFormat="1" ht="52">
-      <c r="A45" s="24" t="s">
+    <row r="45" spans="1:8" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="18">
         <v>43</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="E45" s="9">
+      <c r="D45" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E45" s="7">
         <v>42214</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F45" s="7">
         <v>42220</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="7">
         <v>42221</v>
       </c>
-      <c r="H45" s="19" t="s">
+      <c r="H45" s="17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="19" customFormat="1" ht="26">
-      <c r="A46" s="19" t="s">
+    <row r="46" spans="1:8" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="20">
+      <c r="B46" s="18">
         <v>44</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="E46" s="9">
+      <c r="D46" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E46" s="7">
         <v>42214</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46" s="7">
         <v>42220</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="7">
         <v>42221</v>
       </c>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="17" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A47" s="17" t="s">
+    <row r="47" spans="1:8" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="20">
+      <c r="B47" s="18">
         <v>45</v>
       </c>
-      <c r="C47" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" s="9">
+      <c r="C47" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E47" s="7">
         <v>42219</v>
       </c>
-      <c r="F47" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G47" s="9">
+      <c r="F47" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G47" s="7">
         <v>42221</v>
       </c>
-      <c r="H47" s="17">
+      <c r="H47" s="15">
         <v>6137</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="20" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A48" s="20" t="s">
+    <row r="48" spans="1:8" s="18" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="20">
+      <c r="B48" s="18">
         <v>46</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="E48" s="9">
+      <c r="C48" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" s="7">
         <v>42221</v>
       </c>
-      <c r="F48" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="9">
+      <c r="F48" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48" s="7">
         <v>42221</v>
       </c>
-      <c r="H48" s="20">
+      <c r="H48" s="18">
         <v>6137</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="21" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A49" s="21" t="s">
+    <row r="49" spans="1:9" s="19" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="21">
+      <c r="B49" s="19">
         <v>47</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D49" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E49" s="9">
+      <c r="D49" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E49" s="7">
         <v>42222</v>
       </c>
-      <c r="F49" s="9">
+      <c r="F49" s="7">
         <v>42222</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="7">
         <v>42222</v>
       </c>
-      <c r="H49" s="21">
+      <c r="H49" s="19">
         <v>6142</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="26">
-      <c r="A50" s="20" t="s">
+    <row r="50" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="21">
+      <c r="B50" s="19">
         <v>48</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E50" s="9">
+      <c r="D50" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" s="7">
         <v>42221</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F50" s="7">
         <v>42222</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="7">
         <v>42222</v>
       </c>
-      <c r="H50" s="21">
+      <c r="H50" s="19">
         <v>6145</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="52">
-      <c r="A51" s="11" t="s">
+    <row r="51" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B51" s="21">
+      <c r="B51" s="19">
         <v>49</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E51" s="9">
+      <c r="D51" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E51" s="7">
         <v>42222</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="7">
         <v>42222</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="7">
         <v>42222</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H51" s="9">
         <v>6145</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="54" customHeight="1">
-      <c r="A52" s="22" t="s">
+    <row r="52" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="22">
+      <c r="B52" s="20">
         <v>50</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="E52" s="9">
+      <c r="C52" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="7">
         <v>42222</v>
       </c>
-      <c r="F52" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="G52" s="9">
+      <c r="F52" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" s="7">
         <v>42222</v>
       </c>
-      <c r="H52" s="22" t="s">
+      <c r="H52" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="I52" s="22"/>
-    </row>
-    <row r="53" spans="1:9" ht="39">
-      <c r="A53" s="11" t="s">
+      <c r="I52" s="20"/>
+    </row>
+    <row r="53" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="9">
         <v>51</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E53" s="9">
+      <c r="C53" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E53" s="7">
         <v>42223</v>
       </c>
-      <c r="F53" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G53" s="9">
+      <c r="F53" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G53" s="7">
         <v>42223</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H53" s="9" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="23" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="9">
         <v>52</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E54" s="9">
+      <c r="C54" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="7">
         <v>42223</v>
       </c>
-      <c r="F54" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G54" s="9">
+      <c r="F54" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="7">
         <v>42223</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H54" s="9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="39">
-      <c r="A55" s="11" t="s">
+    <row r="55" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55" s="9">
         <v>53</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E55" s="9">
+      <c r="C55" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" s="7">
         <v>42223</v>
       </c>
-      <c r="F55" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G55" s="9">
+      <c r="F55" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="7">
         <v>42223</v>
       </c>
-      <c r="H55" s="11" t="s">
+      <c r="H55" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="49.5" customHeight="1">
-      <c r="A56" s="11" t="s">
+    <row r="56" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="11">
+      <c r="B56" s="9">
         <v>54</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E56" s="9">
+      <c r="C56" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="7">
         <v>42227</v>
       </c>
-      <c r="F56" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G56" s="9">
+      <c r="F56" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G56" s="7">
         <v>42227</v>
       </c>
-      <c r="H56" s="11" t="s">
+      <c r="H56" s="9" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="26">
-      <c r="A57" s="24" t="s">
+    <row r="57" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B57" s="11">
+      <c r="B57" s="9">
         <v>55</v>
       </c>
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D57" s="24" t="s">
+      <c r="D57" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="7">
         <v>42233</v>
       </c>
-      <c r="F57" s="9">
+      <c r="F57" s="7">
         <v>42234</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="7">
         <v>42234</v>
       </c>
-      <c r="H57" s="11">
+      <c r="H57" s="9">
         <v>6224</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="52">
-      <c r="A58" s="25" t="s">
+    <row r="58" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A58" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B58" s="9">
         <v>56</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D58" s="24" t="s">
+      <c r="D58" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="7">
         <v>42233</v>
       </c>
-      <c r="F58" s="9">
+      <c r="F58" s="7">
         <v>42234</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="7">
         <v>42234</v>
       </c>
-      <c r="H58" s="25" t="s">
+      <c r="H58" s="23" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="11" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59" s="9">
         <v>57</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D59" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E59" s="9">
+      <c r="D59" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E59" s="7">
         <v>42235</v>
       </c>
-      <c r="F59" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G59" s="9">
+      <c r="F59" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G59" s="7">
         <v>42235</v>
       </c>
-      <c r="H59" s="11">
+      <c r="H59" s="9">
         <v>6230</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="26">
-      <c r="A60" s="27" t="s">
+    <row r="60" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B60" s="11">
+      <c r="B60" s="9">
         <v>58</v>
       </c>
-      <c r="C60" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E60" s="9">
+      <c r="C60" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E60" s="7">
         <v>42240</v>
       </c>
-      <c r="F60" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G60" s="9">
+      <c r="F60" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G60" s="7">
         <v>42240</v>
       </c>
-      <c r="H60" s="11">
+      <c r="H60" s="9">
         <v>6254</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="44.25" customHeight="1">
-      <c r="A61" s="11" t="s">
+    <row r="61" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B61" s="11">
+      <c r="B61" s="9">
         <v>59</v>
       </c>
-      <c r="C61" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E61" s="9">
+      <c r="C61" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E61" s="7">
         <v>42240</v>
       </c>
-      <c r="F61" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G61" s="9">
+      <c r="F61" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G61" s="7">
         <v>42240</v>
       </c>
-      <c r="H61" s="11">
+      <c r="H61" s="9">
         <v>6258</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="33" customHeight="1">
-      <c r="A62" s="28" t="s">
+    <row r="62" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B62" s="11">
+      <c r="B62" s="9">
         <v>60</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C62" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="7">
         <v>42240</v>
       </c>
-      <c r="F62" s="28" t="s">
+      <c r="F62" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G62" s="7">
         <v>42240</v>
       </c>
-      <c r="H62" s="11">
+      <c r="H62" s="9">
         <v>6260</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="11" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B63" s="11">
+      <c r="B63" s="9">
         <v>61</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D63" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E63" s="9">
+      <c r="D63" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E63" s="7">
         <v>42240</v>
       </c>
-      <c r="F63" s="29" t="s">
+      <c r="F63" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="7">
         <v>42240</v>
       </c>
-      <c r="H63" s="11">
+      <c r="H63" s="9">
         <v>6263</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="26">
-      <c r="A64" s="31"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="11" t="s">
+    <row r="64" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="11" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B65" s="9">
         <v>60</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D65" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E65" s="9">
+      <c r="D65" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E65" s="7">
         <v>42244</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G65" s="7">
         <v>42244</v>
       </c>
-      <c r="H65" s="11" t="s">
+      <c r="H65" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="11" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="11">
+      <c r="B66" s="9">
         <v>62</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E66" s="9">
+      <c r="D66" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E66" s="7">
         <v>42247</v>
       </c>
-      <c r="F66" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G66" s="9">
+      <c r="F66" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G66" s="7">
         <v>42247</v>
       </c>
-      <c r="H66" s="11">
+      <c r="H66" s="9">
         <v>4611149</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="11" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B67" s="11">
+      <c r="B67" s="9">
         <v>63</v>
       </c>
-      <c r="C67" s="32" t="s">
+      <c r="C67" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D67" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E67" s="9">
+      <c r="D67" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E67" s="7">
         <v>42247</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="7">
         <v>42247</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B68" s="11">
+      <c r="B68" s="9">
         <v>64</v>
       </c>
-      <c r="C68" s="30" t="s">
+      <c r="C68" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D68" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E68" s="7">
         <v>42247</v>
       </c>
-      <c r="F68" s="30" t="s">
+      <c r="F68" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="7">
         <v>42249</v>
       </c>
-      <c r="H68" s="30" t="s">
+      <c r="H68" s="28" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="33" customFormat="1" ht="26">
-      <c r="A69" s="33" t="s">
+    <row r="69" spans="1:8" s="31" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="33">
+      <c r="B69" s="31">
         <v>65</v>
       </c>
-      <c r="C69" s="33" t="s">
+      <c r="C69" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D69" s="33" t="s">
+      <c r="D69" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="E69" s="9">
+      <c r="E69" s="7">
         <v>42258</v>
       </c>
-      <c r="F69" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G69" s="9">
+      <c r="F69" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G69" s="7">
         <v>42258</v>
       </c>
-      <c r="H69" s="33" t="s">
+      <c r="H69" s="31" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="39">
-      <c r="A70" s="11" t="s">
+    <row r="70" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B70" s="11">
+      <c r="B70" s="9">
         <v>66</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E70" s="9">
+      <c r="C70" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E70" s="7">
         <v>42262</v>
       </c>
-      <c r="F70" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G70" s="9">
+      <c r="F70" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G70" s="7">
         <v>42262</v>
       </c>
-      <c r="H70" s="32">
+      <c r="H70" s="30">
         <v>8768403</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="11" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="11">
+      <c r="B71" s="9">
         <v>67</v>
       </c>
-      <c r="C71" s="32" t="s">
+      <c r="C71" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D71" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="E71" s="9">
+      <c r="D71" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="E71" s="7">
         <v>42269</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="7">
         <v>42269</v>
       </c>
-      <c r="H71" s="11" t="s">
+      <c r="H71" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="11" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B72" s="11">
+      <c r="B72" s="9">
         <v>68</v>
       </c>
-      <c r="C72" s="32" t="s">
+      <c r="C72" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D72" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="E72" s="9">
+      <c r="D72" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="E72" s="7">
         <v>42269</v>
       </c>
-      <c r="G72" s="36">
+      <c r="G72" s="34">
         <v>42269</v>
       </c>
-      <c r="H72" s="34" t="s">
+      <c r="H72" s="32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="11" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="11">
+      <c r="B73" s="9">
         <v>69</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D73" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E73" s="9">
+      <c r="D73" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E73" s="7">
         <v>42269</v>
       </c>
-      <c r="F73" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G73" s="9">
+      <c r="F73" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G73" s="7">
         <v>42269</v>
       </c>
-      <c r="H73" s="33" t="s">
+      <c r="H73" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="26">
-      <c r="A74" s="11" t="s">
+    <row r="74" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="11">
+      <c r="B74" s="9">
         <v>70</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D74" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="E74" s="9">
+      <c r="D74" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="E74" s="7">
         <v>42272</v>
       </c>
-      <c r="F74" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G74" s="9">
+      <c r="F74" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G74" s="7">
         <v>42272</v>
       </c>
-      <c r="H74" s="11" t="s">
+      <c r="H74" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="11" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B75" s="35">
+      <c r="B75" s="33">
         <v>71</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D75" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="E75" s="9">
+      <c r="D75" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" s="7">
         <v>42273</v>
       </c>
-      <c r="F75" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G75" s="9">
+      <c r="F75" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G75" s="7">
         <v>42273</v>
       </c>
-      <c r="H75" s="11" t="s">
+      <c r="H75" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="26">
-      <c r="A76" s="11" t="s">
+    <row r="76" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B76" s="35">
+      <c r="B76" s="33">
         <v>72</v>
       </c>
-      <c r="C76" s="35" t="s">
+      <c r="C76" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="D76" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="E76" s="9">
+      <c r="D76" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="E76" s="7">
         <v>42274</v>
       </c>
-      <c r="F76" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G76" s="9">
+      <c r="F76" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G76" s="7">
         <v>42274</v>
       </c>
-      <c r="H76" s="11" t="s">
+      <c r="H76" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="11" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B77" s="37">
+      <c r="B77" s="35">
         <v>73</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D77" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="E77" s="9">
+      <c r="D77" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="7">
         <v>42275</v>
       </c>
-      <c r="F77" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G77" s="9">
+      <c r="F77" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G77" s="7">
         <v>42275</v>
       </c>
-      <c r="H77" s="11" t="s">
+      <c r="H77" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="26">
-      <c r="A78" s="11" t="s">
+    <row r="78" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B78" s="37">
+      <c r="B78" s="35">
         <v>74</v>
       </c>
-      <c r="C78" s="37" t="s">
+      <c r="C78" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D78" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="E78" s="9">
+      <c r="D78" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="E78" s="7">
         <v>42275</v>
       </c>
-      <c r="F78" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G78" s="9">
+      <c r="F78" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G78" s="7">
         <v>42275</v>
       </c>
-      <c r="H78" s="11" t="s">
+      <c r="H78" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="26">
-      <c r="A79" s="11" t="s">
+    <row r="79" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="37">
+      <c r="B79" s="35">
         <v>75</v>
       </c>
-      <c r="C79" s="37" t="s">
+      <c r="C79" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D79" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="E79" s="9">
+      <c r="D79" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="E79" s="7">
         <v>42275</v>
       </c>
-      <c r="F79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G79" s="9">
+      <c r="F79" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G79" s="7">
         <v>42275</v>
       </c>
-      <c r="H79" s="11" t="s">
+      <c r="H79" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="11" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B80" s="37">
+      <c r="B80" s="35">
         <v>76</v>
       </c>
-      <c r="C80" s="38" t="s">
+      <c r="C80" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D80" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E80" s="9">
+      <c r="D80" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="E80" s="7">
         <v>42275</v>
       </c>
-      <c r="F80" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="G80" s="9">
+      <c r="F80" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="G80" s="7">
         <v>42275</v>
       </c>
-      <c r="H80" s="11" t="s">
+      <c r="H80" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="39">
-      <c r="A81" s="11" t="s">
+    <row r="81" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B81" s="11">
+      <c r="B81" s="9">
         <v>77</v>
       </c>
-      <c r="C81" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E81" s="9">
+      <c r="C81" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E81" s="7">
         <v>42276</v>
       </c>
-      <c r="F81" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G81" s="9">
+      <c r="F81" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G81" s="7">
         <v>42276</v>
       </c>
-      <c r="H81" s="11" t="s">
+      <c r="H81" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="44" customFormat="1">
-      <c r="A82" s="44" t="s">
+    <row r="82" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B82" s="44">
+      <c r="B82" s="42">
         <v>78</v>
       </c>
-      <c r="C82" s="44" t="s">
+      <c r="C82" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D82" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E82" s="9">
+      <c r="D82" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E82" s="7">
         <v>42278</v>
       </c>
-      <c r="G82" s="9">
+      <c r="G82" s="7">
         <v>42278</v>
       </c>
-      <c r="H82" s="44" t="s">
+      <c r="H82" s="42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="44" customFormat="1">
-      <c r="A83" s="44" t="s">
+    <row r="83" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B83" s="44">
+      <c r="B83" s="42">
         <v>79</v>
       </c>
-      <c r="C83" s="44" t="s">
+      <c r="C83" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D83" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E83" s="9">
+      <c r="D83" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E83" s="7">
         <v>42278</v>
       </c>
-      <c r="G83" s="9">
+      <c r="G83" s="7">
         <v>42278</v>
       </c>
-      <c r="H83" s="44" t="s">
+      <c r="H83" s="42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="44" customFormat="1">
-      <c r="A84" s="44" t="s">
+    <row r="84" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B84" s="44">
+      <c r="B84" s="42">
         <v>80</v>
       </c>
-      <c r="C84" s="44" t="s">
+      <c r="C84" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D84" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E84" s="9">
+      <c r="D84" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E84" s="7">
         <v>42278</v>
       </c>
-      <c r="G84" s="9">
+      <c r="G84" s="7">
         <v>42278</v>
       </c>
-      <c r="H84" s="44" t="s">
+      <c r="H84" s="42" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="44" customFormat="1" ht="26">
-      <c r="A85" s="44" t="s">
+    <row r="85" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B85" s="44">
+      <c r="B85" s="42">
         <v>81</v>
       </c>
-      <c r="C85" s="44" t="s">
+      <c r="C85" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E85" s="9">
+      <c r="D85" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E85" s="7">
         <v>42282</v>
       </c>
-      <c r="G85" s="9">
+      <c r="G85" s="7">
         <v>42282</v>
       </c>
-      <c r="H85" s="44" t="s">
+      <c r="H85" s="42" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="44" customFormat="1" ht="26">
-      <c r="A86" s="44" t="s">
+    <row r="86" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B86" s="44">
+      <c r="B86" s="42">
         <v>82</v>
       </c>
-      <c r="C86" s="44" t="s">
+      <c r="C86" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D86" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E86" s="9">
+      <c r="D86" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E86" s="7">
         <v>42290</v>
       </c>
-      <c r="G86" s="9">
+      <c r="G86" s="7">
         <v>42290</v>
       </c>
-      <c r="H86" s="44" t="s">
+      <c r="H86" s="42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="44" customFormat="1">
-      <c r="A87" s="44" t="s">
+    <row r="87" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B87" s="44">
+      <c r="B87" s="42">
         <v>83</v>
       </c>
-      <c r="C87" s="44" t="s">
+      <c r="C87" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D87" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E87" s="9">
+      <c r="D87" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E87" s="7">
         <v>42321</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="7">
         <v>42321</v>
       </c>
-      <c r="H87" s="44" t="s">
+      <c r="H87" s="42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="44" customFormat="1" ht="65">
-      <c r="A88" s="44" t="s">
+    <row r="88" spans="1:8" s="42" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B88" s="44">
+      <c r="B88" s="42">
         <v>84</v>
       </c>
-      <c r="C88" s="44" t="s">
+      <c r="C88" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D88" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E88" s="9">
+      <c r="D88" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E88" s="7">
         <v>42321</v>
       </c>
-      <c r="G88" s="9">
+      <c r="G88" s="7">
         <v>42321</v>
       </c>
-      <c r="H88" s="44" t="s">
+      <c r="H88" s="42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="26">
-      <c r="A89" s="11" t="s">
+    <row r="89" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B89" s="44">
+      <c r="B89" s="42">
         <v>85</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D89" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E89" s="9">
+      <c r="D89" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E89" s="7">
         <v>42293</v>
       </c>
-      <c r="F89" s="9">
+      <c r="F89" s="7">
         <v>42300</v>
       </c>
-      <c r="G89" s="9">
+      <c r="G89" s="7">
         <v>42300</v>
       </c>
-      <c r="H89" s="39" t="s">
+      <c r="H89" s="37" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="39">
-      <c r="A90" s="11" t="s">
+    <row r="90" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B90" s="44">
+      <c r="B90" s="42">
         <v>86</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C90" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D90" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="E90" s="36">
+      <c r="D90" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E90" s="34">
         <v>42300</v>
       </c>
-      <c r="F90" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G90" s="9">
+      <c r="F90" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G90" s="7">
         <v>42300</v>
       </c>
-      <c r="H90" s="11" t="s">
+      <c r="H90" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="39">
-      <c r="A91" s="11" t="s">
+    <row r="91" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="44">
+      <c r="B91" s="42">
         <v>87</v>
       </c>
-      <c r="C91" s="40" t="s">
+      <c r="C91" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="D91" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="E91" s="36">
+      <c r="D91" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E91" s="34">
         <v>42300</v>
       </c>
-      <c r="F91" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G91" s="36">
+      <c r="F91" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G91" s="34">
         <v>42300</v>
       </c>
-      <c r="H91" s="40" t="s">
+      <c r="H91" s="38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="39">
-      <c r="A92" s="42" t="s">
+    <row r="92" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B92" s="44">
+      <c r="B92" s="42">
         <v>88</v>
       </c>
-      <c r="C92" s="41" t="s">
+      <c r="C92" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D92" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="E92" s="9">
+      <c r="D92" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="E92" s="7">
         <v>42321</v>
       </c>
-      <c r="F92" s="41" t="s">
+      <c r="F92" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G92" s="9">
+      <c r="G92" s="7">
         <v>42321</v>
       </c>
-      <c r="H92" s="41" t="s">
+      <c r="H92" s="39" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="26">
-      <c r="A93" s="43" t="s">
+    <row r="93" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="B93" s="44">
+      <c r="B93" s="42">
         <v>89</v>
       </c>
-      <c r="C93" s="43" t="s">
+      <c r="C93" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D93" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="E93" s="9">
+      <c r="D93" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="E93" s="7">
         <v>42321</v>
       </c>
-      <c r="F93" s="43" t="s">
+      <c r="F93" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G93" s="9">
+      <c r="G93" s="7">
         <v>42321</v>
       </c>
-      <c r="H93" s="43" t="s">
+      <c r="H93" s="41" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="44" customFormat="1" ht="39">
-      <c r="A94" s="44" t="s">
+    <row r="94" spans="1:8" s="42" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A94" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="44">
+      <c r="B94" s="42">
         <v>90</v>
       </c>
-      <c r="C94" s="44" t="s">
+      <c r="C94" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D94" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E94" s="9">
+      <c r="D94" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E94" s="7">
         <v>42339</v>
       </c>
-      <c r="G94" s="9">
+      <c r="G94" s="7">
         <v>42339</v>
       </c>
-      <c r="H94" s="44" t="s">
+      <c r="H94" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="11" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B95" s="45">
+      <c r="B95" s="43">
         <v>91</v>
       </c>
-      <c r="C95" s="45" t="s">
+      <c r="C95" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D95" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="E95" s="9">
+      <c r="D95" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E95" s="7">
         <v>42342</v>
       </c>
-      <c r="G95" s="9">
+      <c r="G95" s="7">
         <v>42342</v>
       </c>
-      <c r="H95" s="45" t="s">
+      <c r="H95" s="43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="11" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B96" s="45">
+      <c r="B96" s="43">
         <v>92</v>
       </c>
-      <c r="C96" s="45" t="s">
+      <c r="C96" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D96" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="E96" s="9">
+      <c r="D96" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E96" s="7">
         <v>42345</v>
       </c>
-      <c r="G96" s="9">
+      <c r="G96" s="7">
         <v>42345</v>
       </c>
-      <c r="H96" s="45" t="s">
+      <c r="H96" s="43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="45" t="s">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B97" s="45">
+      <c r="B97" s="43">
         <v>93</v>
       </c>
-      <c r="C97" s="45" t="s">
+      <c r="C97" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D97" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="E97" s="9">
+      <c r="D97" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E97" s="7">
         <v>42346</v>
       </c>
-      <c r="G97" s="9">
+      <c r="G97" s="7">
         <v>42346</v>
       </c>
-      <c r="H97" s="45" t="s">
+      <c r="H97" s="43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="26">
-      <c r="A98" s="11" t="s">
+    <row r="98" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B98" s="11">
+      <c r="B98" s="9">
         <v>94</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D98" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E98" s="9">
+      <c r="D98" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E98" s="7">
         <v>42355</v>
       </c>
-      <c r="F98" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="G98" s="9">
+      <c r="F98" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G98" s="7">
         <v>42359</v>
       </c>
-      <c r="H98" s="46" t="s">
+      <c r="H98" s="44" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="99" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B99" s="9">
+        <v>95</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E99" s="7">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B100" s="9">
+        <v>96</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E100" s="7">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:G1"/>

</xml_diff>

<commit_message>
Update to code change tracker- you guys really should still be using this
</commit_message>
<xml_diff>
--- a/documentation/CEDS_Code_Change_Tracker.xlsx
+++ b/documentation/CEDS_Code_Change_Tracker.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="177">
   <si>
     <t>Remove automaticall install libraries</t>
   </si>
@@ -589,15 +589,6 @@
     <t>ed989b7</t>
   </si>
   <si>
-    <t>Added instantiation of "scripts" variable before conditionals to determine child scripts to execute in F1.1.inventory_scaling.R, to avoid errors during execution for BC emissions</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Created C1.2.add_NC_emissions_EDGAR.R to process and add EDGAR default emissions data for various emissions species to their respective default emissions databases, added call to new script into C1.2.add_NC_emissions.R.</t>
   </si>
   <si>
@@ -608,6 +599,15 @@
   </si>
   <si>
     <t>Created NC_EDGAR_sector_mapping.csv and Master_EDGAR_sector_mapping.csv for use in module C and checking presence of all EDGAR sectors in final emissions database.</t>
+  </si>
+  <si>
+    <t>Upgraded IO_functions.R readData function to include ability to read one, all, or a select list of .csv files from within a .zip file. Added listZippedFiles function.</t>
+  </si>
+  <si>
+    <t>Renamed E.UNFCCC_SO2_emissions.R to E.UNFCCC_emissions.R, updated to use new readData .zip features to read all data from within large .zip files, added dummy output for species without present input data.</t>
+  </si>
+  <si>
+    <t>ce6f6a3</t>
   </si>
 </sst>
 </file>
@@ -718,7 +718,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -824,6 +824,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1200,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E107" sqref="E107"/>
+      <selection pane="bottomLeft" activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1219,15 +1222,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3692,28 +3695,37 @@
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B99" s="9">
+      <c r="B99" s="45">
         <v>95</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>123</v>
       </c>
       <c r="D99" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E99" s="7">
+        <v>42377</v>
+      </c>
+      <c r="F99" s="7">
+        <v>42377</v>
+      </c>
+      <c r="G99" s="7">
+        <v>42377</v>
+      </c>
+      <c r="H99" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E99" s="7">
-        <v>42373</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B100" s="9">
+      <c r="B100" s="45">
         <v>96</v>
       </c>
       <c r="C100" s="9" t="s">
@@ -3723,52 +3735,97 @@
         <v>153</v>
       </c>
       <c r="E100" s="7">
-        <v>42377</v>
+        <v>42380</v>
       </c>
       <c r="F100" s="7">
-        <v>42377</v>
+        <v>42016</v>
       </c>
       <c r="G100" s="7">
-        <v>42377</v>
-      </c>
-      <c r="H100" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42017</v>
+      </c>
+      <c r="H100" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B101" s="9">
+        <v>171</v>
+      </c>
+      <c r="B101" s="45">
         <v>97</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>123</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="E101" s="7">
         <v>42380</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F101" s="7">
+        <v>42016</v>
+      </c>
+      <c r="G101" s="7">
+        <v>42017</v>
+      </c>
+      <c r="H101" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B102" s="9">
+      <c r="B102" s="45">
         <v>98</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>123</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="E102" s="7">
-        <v>42380</v>
-      </c>
-    </row>
+        <v>42384</v>
+      </c>
+      <c r="F102" s="7">
+        <v>42387</v>
+      </c>
+      <c r="G102" s="7">
+        <v>42387</v>
+      </c>
+      <c r="H102" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B103" s="45">
+        <v>99</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E103" s="7">
+        <v>42384</v>
+      </c>
+      <c r="F103" s="7">
+        <v>42387</v>
+      </c>
+      <c r="G103" s="7">
+        <v>42387</v>
+      </c>
+      <c r="H103" s="45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>

</xml_diff>